<commit_message>
Almost done with WHY section
</commit_message>
<xml_diff>
--- a/assets/DevVsMaintCostChart.xlsx
+++ b/assets/DevVsMaintCostChart.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
   <si>
     <t>Quarters</t>
   </si>
@@ -91,8 +91,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -115,7 +119,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -125,6 +129,8 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -134,6 +140,8 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -348,34 +356,34 @@
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>4.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
                   <c:v>7.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>10.0</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>16.0</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>23.0</c:v>
+                  <c:v>14.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>34.0</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45.0</c:v>
+                  <c:v>28.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>55.0</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>65.0</c:v>
+                  <c:v>33.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>75.0</c:v>
+                  <c:v>33.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -389,11 +397,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2135592680"/>
-        <c:axId val="2135876344"/>
+        <c:axId val="2081821336"/>
+        <c:axId val="2081824312"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="2135592680"/>
+        <c:axId val="2081821336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -402,7 +410,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2135876344"/>
+        <c:crossAx val="2081824312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -410,7 +418,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2135876344"/>
+        <c:axId val="2081824312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -421,7 +429,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2135592680"/>
+        <c:crossAx val="2081821336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -810,10 +818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -870,7 +878,7 @@
         <v>20</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -881,7 +889,7 @@
         <v>10</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -892,7 +900,7 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -903,7 +911,7 @@
         <v>4</v>
       </c>
       <c r="C8">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -914,7 +922,7 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -925,7 +933,7 @@
         <v>2</v>
       </c>
       <c r="C10">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -936,7 +944,7 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -947,7 +955,7 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>55</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -958,7 +966,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>65</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -969,6 +977,17 @@
         <v>0</v>
       </c>
       <c r="C14">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
         <v>75</v>
       </c>
     </row>

</xml_diff>